<commit_message>
added shrink fit analysis to a second sheet on the shrink fit calc document
</commit_message>
<xml_diff>
--- a/Analysis/Calculations/shrink_fit_calc.xlsx
+++ b/Analysis/Calculations/shrink_fit_calc.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\russt\Desktop\GIT\composite-propellant-tank\Analysis\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18260" windowHeight="9040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18264" windowHeight="9036" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Di,final</t>
   </si>
@@ -60,6 +61,101 @@
   </si>
   <si>
     <t>t, initial</t>
+  </si>
+  <si>
+    <t>DELTA Do</t>
+  </si>
+  <si>
+    <t>Delta Max</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>Poisson's Ratio</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>PTFE</t>
+  </si>
+  <si>
+    <r>
+      <t>CTE (in/in/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°F)</t>
+    </r>
+  </si>
+  <si>
+    <t>Elastic Modulus (psi)</t>
+  </si>
+  <si>
+    <t>Temperature Change</t>
+  </si>
+  <si>
+    <t>Inner Radius</t>
+  </si>
+  <si>
+    <t>Ring Dimensions</t>
+  </si>
+  <si>
+    <t>Outer Radius</t>
+  </si>
+  <si>
+    <t>Cap Dimensions</t>
+  </si>
+  <si>
+    <t>(inches)</t>
+  </si>
+  <si>
+    <t>Liner Dimensions</t>
+  </si>
+  <si>
+    <t>Aluminum Interface Pressure (psi)</t>
+  </si>
+  <si>
+    <t>Liner Pressure at Cryo Temp (psi)</t>
+  </si>
+  <si>
+    <t>Interface Depth</t>
+  </si>
+  <si>
+    <t>Interface Area (in^2)</t>
+  </si>
+  <si>
+    <t>Total Force (lb)</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Cryo Thickness</t>
+  </si>
+  <si>
+    <t>Change in Thickness</t>
+  </si>
+  <si>
+    <t>Fluid Pressure on Cap (psi)</t>
+  </si>
+  <si>
+    <t>Normal Force (lb)</t>
+  </si>
+  <si>
+    <t>Friction Force (lb)</t>
+  </si>
+  <si>
+    <t>Friction Coefficient</t>
   </si>
 </sst>
 </file>
@@ -69,13 +165,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -426,25 +528,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:N34"/>
+  <dimension ref="D4:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.26953125" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -452,8 +554,14 @@
         <f>-321-65</f>
         <v>-386</v>
       </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="6" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>8</v>
       </c>
@@ -462,7 +570,7 @@
         <v>1.3099999999999998E-5</v>
       </c>
     </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
@@ -484,6 +592,9 @@
       <c r="J8" t="s">
         <v>6</v>
       </c>
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
       <c r="L8" t="s">
         <v>4</v>
       </c>
@@ -493,22 +604,24 @@
       <c r="N8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.35">
+      <c r="P8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D9">
-        <v>2.5</v>
+        <v>2.875</v>
       </c>
       <c r="E9" s="5">
-        <f>D9+0.5</f>
+        <f>D9+F9</f>
         <v>3</v>
       </c>
       <c r="F9">
-        <f>E9-D9</f>
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="G9" s="2">
         <f>D9+$E$6*$E$5*D9</f>
-        <v>2.4873585</v>
+        <v>2.8604622750000002</v>
       </c>
       <c r="H9" s="6">
         <f>E9+E6*(E5)*E9</f>
@@ -516,25 +629,33 @@
       </c>
       <c r="I9" s="2">
         <f>H9-G9</f>
-        <v>0.49747170000000018</v>
+        <v>0.12436792500000005</v>
       </c>
       <c r="J9" s="2">
         <f>F9-I9</f>
-        <v>2.5282999999998168E-3</v>
+        <v>6.320749999999542E-4</v>
+      </c>
+      <c r="K9" s="2">
+        <f>E9-H9</f>
+        <v>1.5169799999999789E-2</v>
       </c>
       <c r="L9">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="M9" s="2">
         <f>L9+13.1*10^-6*(-386)*L9</f>
-        <v>0.49747170000000002</v>
+        <v>0.124367925</v>
       </c>
       <c r="N9" s="2">
         <f>L9-M9</f>
-        <v>2.5282999999999833E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.35">
+        <v>6.3207499999999583E-4</v>
+      </c>
+      <c r="P9">
+        <f>K9/2</f>
+        <v>7.5848999999998945E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -542,7 +663,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -550,7 +671,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>10</v>
       </c>
@@ -561,7 +682,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>7</v>
       </c>
@@ -576,7 +697,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>8</v>
       </c>
@@ -591,7 +712,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -599,7 +720,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>2</v>
       </c>
@@ -622,7 +743,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D17" s="1">
         <v>2.9</v>
       </c>
@@ -650,7 +771,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D18">
         <v>2.91</v>
       </c>
@@ -667,7 +788,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D19">
         <v>2.92</v>
       </c>
@@ -684,7 +805,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D20" s="1">
         <v>2.93</v>
       </c>
@@ -701,7 +822,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D21">
         <v>2.94</v>
       </c>
@@ -718,7 +839,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D22">
         <v>2.95</v>
       </c>
@@ -735,7 +856,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D23" s="1">
         <v>2.96</v>
       </c>
@@ -752,7 +873,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D24">
         <v>2.97</v>
       </c>
@@ -769,7 +890,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D25" s="5">
         <v>2.98</v>
       </c>
@@ -786,7 +907,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D26" s="1">
         <v>2.99</v>
       </c>
@@ -803,7 +924,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -811,7 +932,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -819,7 +940,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -827,7 +948,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -836,7 +957,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -844,7 +965,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -852,7 +973,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="7:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -860,7 +981,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="7:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -872,4 +993,249 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:J24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <f>0.0000131</f>
+        <v>1.31E-5</v>
+      </c>
+      <c r="E3">
+        <f>0.000086*(5/9)</f>
+        <v>4.7777777777777784E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>10000000</v>
+      </c>
+      <c r="E4">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>0.33</v>
+      </c>
+      <c r="E5">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <f>(9/5)*(293-77)</f>
+        <v>388.8</v>
+      </c>
+      <c r="E6">
+        <f>D6</f>
+        <v>388.8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>1.5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
+        <f>G10-0.125</f>
+        <v>1.375</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9">
+        <f>D9</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10">
+        <f>D9</f>
+        <v>1.5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <f>J9+0.125</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>0.125</v>
+      </c>
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11">
+        <f>0.125</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <f>2*3.141592*D9*D11</f>
+        <v>1.1780970000000002</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12">
+        <f>J11-J11*E3*E6</f>
+        <v>0.122678</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13">
+        <f>J11-J12</f>
+        <v>2.3220000000000046E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f>(D4*Sheet1!P9)/(2*D9^3)*((D10^2-D9^2)*(D9^2-G9^2)/(D10^2-G9^2))</f>
+        <v>3350.2576131686783</v>
+      </c>
+      <c r="D18">
+        <f>C18*D12</f>
+        <v>3946.9284433011808</v>
+      </c>
+      <c r="E18">
+        <v>1.2</v>
+      </c>
+      <c r="F18">
+        <f>E18*D18</f>
+        <v>4736.3141319614169</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f>(((Sheet1!P9-J13)/2)/(J12))*E4</f>
+        <v>10725.028122401511</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>45</v>
+      </c>
+      <c r="D24">
+        <f>C24*3.141592*D9^2</f>
+        <v>318.08619000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more analysis to the shrink fit document
</commit_message>
<xml_diff>
--- a/Analysis/Calculations/shrink_fit_calc.xlsx
+++ b/Analysis/Calculations/shrink_fit_calc.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Di,final</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>Friction Coefficient</t>
+  </si>
+  <si>
+    <t>Theoretical</t>
+  </si>
+  <si>
+    <t>Delta Achievable</t>
+  </si>
+  <si>
+    <t>Shear area (in^2)</t>
+  </si>
+  <si>
+    <t>Shear stress (psi)</t>
+  </si>
+  <si>
+    <t>Shear strength</t>
+  </si>
+  <si>
+    <t>FoS*</t>
   </si>
 </sst>
 </file>
@@ -229,6 +247,156 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D83CA324-5E08-4053-AE5A-583A4EA1FBAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="4754880"/>
+          <a:ext cx="7604760" cy="739140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The best possible seal is achieved by loading the PTFE liner to the max it can handle. According to DuPont, PTFE has a yield stress of 19000 psi at cryo temp. We cannot accomplish this kind of pressure from our shrink fit at this tank size, but we know there will be stress concentrations</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> at the ends of the aluminum cylinders that bind the liner, so we do not want to load the liner to 19000 psi anyway. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4833FDCA-E731-4239-8F5B-F2C790E26708}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11902440" y="2918460"/>
+          <a:ext cx="1828800" cy="563880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>*Stress concentrations not accounted for</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:P34"/>
+  <dimension ref="D4:R34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,12 +709,12 @@
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -561,7 +729,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="6" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>8</v>
       </c>
@@ -570,7 +738,12 @@
         <v>1.3099999999999998E-5</v>
       </c>
     </row>
-    <row r="8" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="P7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
@@ -607,8 +780,11 @@
       <c r="P8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D9">
         <v>2.875</v>
       </c>
@@ -654,8 +830,12 @@
         <f>K9/2</f>
         <v>7.5848999999998945E-3</v>
       </c>
-    </row>
-    <row r="10" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <f>P9-0.0025/2</f>
+        <v>6.3348999999998943E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:18" x14ac:dyDescent="0.3">
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -663,7 +843,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:18" x14ac:dyDescent="0.3">
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -671,7 +851,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>10</v>
       </c>
@@ -682,7 +862,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>7</v>
       </c>
@@ -697,7 +877,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>8</v>
       </c>
@@ -712,7 +892,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:18" x14ac:dyDescent="0.3">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -720,7 +900,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>2</v>
       </c>
@@ -997,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J24"/>
+  <dimension ref="C2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1010,6 +1190,8 @@
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.3">
@@ -1175,7 +1357,7 @@
         <v>2.3220000000000046E-3</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>28</v>
       </c>
@@ -1188,36 +1370,63 @@
       <c r="F17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18">
-        <f>(D4*Sheet1!P9)/(2*D9^3)*((D10^2-D9^2)*(D9^2-G9^2)/(D10^2-G9^2))</f>
-        <v>3350.2576131686783</v>
+        <f>(D4*Sheet1!R9)/(2*D9^3)*((D10^2-D9^2)*(D9^2-G9^2)/(D10^2-G9^2))</f>
+        <v>2798.1314128943291</v>
       </c>
       <c r="D18">
         <f>C18*D12</f>
-        <v>3946.9284433011808</v>
+        <v>3296.4702231365709</v>
       </c>
       <c r="E18">
         <v>1.2</v>
       </c>
       <c r="F18">
         <f>E18*D18</f>
-        <v>4736.3141319614169</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+        <v>3955.7642677638851</v>
+      </c>
+      <c r="I18">
+        <f>3.141592*(G10^2-G9^2)</f>
+        <v>1.1290096250000001</v>
+      </c>
+      <c r="J18">
+        <f>D18/I18</f>
+        <v>2919.789300411474</v>
+      </c>
+      <c r="K18">
+        <v>30000</v>
+      </c>
+      <c r="L18">
+        <f>K18/J18</f>
+        <v>10.274713999319136</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21">
-        <f>(((Sheet1!P9-J13)/2)/(J12))*E4</f>
-        <v>10725.028122401511</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+        <f>(((Sheet1!R9-J13)/2)/(J12))*E4</f>
+        <v>8177.7091247002099</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>36</v>
       </c>
@@ -1225,7 +1434,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>45</v>
       </c>
@@ -1237,5 +1446,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>